<commit_message>
user data and updated uganda financial calcs
</commit_message>
<xml_diff>
--- a/user-data/adult-literacy/adult-literacy.xlsx
+++ b/user-data/adult-literacy/adult-literacy.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="457">
   <si>
     <t>id</t>
   </si>
@@ -1376,7 +1376,10 @@
     <t>The following is data downloaded from Development Initiative's Datahub: http://devinit.org/data</t>
   </si>
   <si>
-    <t>It is provided on an as-is basis under an open-use license.</t>
+    <t>It is licensed under a Creative Commons Attribution 4.0 International license.</t>
+  </si>
+  <si>
+    <t>More information on licensing is available here: https://creativecommons.org/licenses/by/4.0/</t>
   </si>
   <si>
     <t>For concerns, questions, or corrections: please email info@devinit.org</t>
@@ -1809,6 +1812,11 @@
         <v>455</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>